<commit_message>
update BOM.xlsx to content of readme.md
</commit_message>
<xml_diff>
--- a/02_Deckbox/01_Hardware/BOM.xlsx
+++ b/02_Deckbox/01_Hardware/BOM.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD49A64F-274E-4481-B3DF-15A9EA6750CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B530254-4359-491B-B379-8E9E31B77AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14508" yWindow="-7908" windowWidth="14616" windowHeight="22536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
   <si>
     <t>#</t>
   </si>
@@ -40,24 +40,12 @@
     <t>pc</t>
   </si>
   <si>
-    <t>Rittal-PK-9548.000 Mounting plate</t>
-  </si>
-  <si>
     <t>for power supply of router</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>to attach router and raspb. to mouting plate (von Andreas)</t>
-  </si>
-  <si>
-    <t>Dremel/ Drilling machine small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reader for micro SD card </t>
-  </si>
-  <si>
     <t>for power supply of Pi</t>
   </si>
   <si>
@@ -76,18 +64,6 @@
     <t>Mounting for box on reeling</t>
   </si>
   <si>
-    <t>Hexagonal screw, M4x16, incl. washer and self-securing nut, stainless steel V4A</t>
-  </si>
-  <si>
-    <t>Steel strap for tubes, DIN 3570, nominal width 46 mm, incl. 2 M10 self-securing nuts and 2 M10 washers, stainless steel V4A</t>
-  </si>
-  <si>
-    <t>Steel strap for tubes, DIN 3570, nominal width 82 mm, incl. 2 M12 self-securing nuts and 2 M12 washers, stainless steel V4A</t>
-  </si>
-  <si>
-    <t>Rittal-PK-9518.000 Case 182x180x111 (Art.-Nr.: W84179)</t>
-  </si>
-  <si>
     <t>External power supply</t>
   </si>
   <si>
@@ -130,12 +106,6 @@
     <t xml:space="preserve">product numbers 0039039042 430300038 </t>
   </si>
   <si>
-    <t>e.g. 4064161155296</t>
-  </si>
-  <si>
-    <t>USB C plug, rectangular, e.g. cut from cable</t>
-  </si>
-  <si>
     <t>2050005621999</t>
   </si>
   <si>
@@ -193,51 +163,18 @@
     <t>for merging incoming power sources</t>
   </si>
   <si>
-    <t>4028177139657</t>
-  </si>
-  <si>
-    <t>4028177140097</t>
-  </si>
-  <si>
-    <t>3D printed mounting for electronic components</t>
-  </si>
-  <si>
     <t>3D printed mounting for antennas of RUT955, consisting of three layers</t>
   </si>
   <si>
     <t>Tools</t>
   </si>
   <si>
-    <t>Drilling machines for 2 mm and 21 mm holes</t>
-  </si>
-  <si>
     <t>e.g. ASIN B09B7F2XM3 or 4260528721160</t>
   </si>
   <si>
-    <t>Threaded inserts to melt into 3D print, M3x6x5</t>
-  </si>
-  <si>
-    <t>Tapping screw (Belchschraube) M2,9x9,5</t>
-  </si>
-  <si>
-    <t>4043377162205</t>
-  </si>
-  <si>
-    <t>Tapping screw (Belchschraube) M2,2x9,5</t>
-  </si>
-  <si>
     <t>4043377159625</t>
   </si>
   <si>
-    <t>Tapping screw (Belchschraube) M3,9x9,5</t>
-  </si>
-  <si>
-    <t>~25</t>
-  </si>
-  <si>
-    <t>Hexagonal screws M3x16</t>
-  </si>
-  <si>
     <t>4043952396568</t>
   </si>
   <si>
@@ -247,12 +184,6 @@
     <t>4043952537589</t>
   </si>
   <si>
-    <t xml:space="preserve">Sealing tape for water tightness </t>
-  </si>
-  <si>
-    <t>Wire 15 cm, 2 x ~0.75mm², red and black</t>
-  </si>
-  <si>
     <t>Soldering station, including equipment e.g. shrinking tubes</t>
   </si>
   <si>
@@ -272,6 +203,133 @@
   </si>
   <si>
     <t>ACDC converter, 12 or 24 V output, min 20 W, e.g. Mean Well LPV-20-12 LED Trafo</t>
+  </si>
+  <si>
+    <t>2-core wire ~25 cm, 2 x ~0.5mm², red and black</t>
+  </si>
+  <si>
+    <t>electric wire ferrule 0.5mm²</t>
+  </si>
+  <si>
+    <t>Heat shrink tubing 20mm x 3mm</t>
+  </si>
+  <si>
+    <t>USB-C Plug, e.g. recable USB C to C plug 5 strands set (consits of 3 parts: plug, housing and heat shrink tubing)</t>
+  </si>
+  <si>
+    <t>FIBOX Case 180x180x150 (Product-No.: 6011323)</t>
+  </si>
+  <si>
+    <t>3D printed mounting for electronic components, consisting of four parts</t>
+  </si>
+  <si>
+    <t>6418074052216</t>
+  </si>
+  <si>
+    <t>Threaded inserts to melt into 3D print, M3x5x4</t>
+  </si>
+  <si>
+    <t>Allen screws M3x16</t>
+  </si>
+  <si>
+    <t>Tapping screw (Belchschraube) M2.9x9.5</t>
+  </si>
+  <si>
+    <t>Tapping screw (Belchschraube) M2.2x6.5</t>
+  </si>
+  <si>
+    <t>Tapping screw (Belchschraube) M3.9x9.5</t>
+  </si>
+  <si>
+    <t>4043377162199</t>
+  </si>
+  <si>
+    <t>(plastic) washers for 3.9 mm with large outer diameter</t>
+  </si>
+  <si>
+    <t>Allen screw, M4x16, incl. washer and self-securing nut, stainless steel V4A</t>
+  </si>
+  <si>
+    <t>Steel strap for tubes, DIN 3570, nominal width 46 mm, incl. 4 M10 nuts and 2 M10 washers, stainless steel V4A</t>
+  </si>
+  <si>
+    <t>Steel strap for tubes, DIN 3570, nominal width 82 mm, incl. 4 M12 nuts and 2 M12 washers, stainless steel V4A</t>
+  </si>
+  <si>
+    <t>Drilling machines 22 mm holes</t>
+  </si>
+  <si>
+    <t>Adapter tip for melting in press nuts</t>
+  </si>
+  <si>
+    <t>Tweezers</t>
+  </si>
+  <si>
+    <t>Diagonal pliers</t>
+  </si>
+  <si>
+    <t>wire stripper</t>
+  </si>
+  <si>
+    <t>Heat gun</t>
+  </si>
+  <si>
+    <t>Wrench 27 mm</t>
+  </si>
+  <si>
+    <t>Allen wrench 2.5 and 3 mm</t>
+  </si>
+  <si>
+    <t>Screwdriver PH1 + PH2</t>
+  </si>
+  <si>
+    <t>Screwdriver flathead (2.5)</t>
+  </si>
+  <si>
+    <t>Caliper</t>
+  </si>
+  <si>
+    <t>Sikaflex (e.g. 291i or some other marine certified adhesive sealant)</t>
+  </si>
+  <si>
+    <t>Spatula</t>
+  </si>
+  <si>
+    <t>Crimp-Tools for 2824-20 and for electric wire ferrules</t>
+  </si>
+  <si>
+    <t>Cleaning equipment: ethanol, q-tips, lint-free wipes</t>
+  </si>
+  <si>
+    <t>flat nose pliers</t>
+  </si>
+  <si>
+    <t>4040849567070</t>
+  </si>
+  <si>
+    <t>9900000247027</t>
+  </si>
+  <si>
+    <t>9900000174064</t>
+  </si>
+  <si>
+    <t>4043952175507</t>
+  </si>
+  <si>
+    <t>4043952665589
+4001796381737</t>
+  </si>
+  <si>
+    <t>4260396830346</t>
+  </si>
+  <si>
+    <t>4043377065032</t>
+  </si>
+  <si>
+    <t>9900000247645</t>
+  </si>
+  <si>
+    <t>~5 cm foam tape (20x2 mm)</t>
   </si>
 </sst>
 </file>
@@ -344,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -378,9 +436,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -661,21 +716,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="4.3984375" customWidth="1"/>
-    <col min="4" max="4" width="64.73046875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="22.3984375" style="15" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="1" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,23 +744,23 @@
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="11" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -716,15 +771,15 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -735,13 +790,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -752,10 +807,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -766,20 +821,20 @@
         <v>5</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="D7" s="11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -790,16 +845,16 @@
         <v>5</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -810,34 +865,34 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -848,10 +903,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -862,63 +917,76 @@
         <v>5</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10</v>
       </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="5"/>
-      <c r="D15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -927,22 +995,20 @@
         <v>5</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="D17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="5"/>
-      <c r="D17" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -951,30 +1017,20 @@
         <v>5</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="6">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="D19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>15</v>
       </c>
@@ -985,13 +1041,13 @@
         <v>5</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>16</v>
       </c>
@@ -1002,13 +1058,13 @@
         <v>5</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>17</v>
       </c>
@@ -1019,22 +1075,32 @@
         <v>5</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="5"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
       <c r="D23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1046,61 +1112,51 @@
         <v>42</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="6">
-        <v>19</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="D25" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>20</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>21</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>22</v>
       </c>
@@ -1111,24 +1167,33 @@
         <v>5</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>23</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
         <v>24</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="6">
-        <v>23</v>
-      </c>
       <c r="B30">
         <v>1</v>
       </c>
@@ -1136,49 +1201,39 @@
         <v>5</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="6">
-        <v>24</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="5">
+        <v>43</v>
+      </c>
+      <c r="E30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
         <v>25</v>
       </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>26</v>
       </c>
       <c r="B33">
@@ -1188,141 +1243,158 @@
         <v>5</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>27</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>28</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>29</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>30</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D37" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>31</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>70</v>
+      <c r="B38">
+        <v>2</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>32</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>33</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="5"/>
-      <c r="D41" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>34</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1330,89 +1402,180 @@
       <c r="C42" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="6">
-        <v>35</v>
-      </c>
-      <c r="B43">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" s="14"/>
-    </row>
-    <row r="44" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="D43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>36</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D44" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>37</v>
       </c>
       <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>38</v>
+      </c>
+      <c r="B46">
         <v>2</v>
       </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="5"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="5"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D51" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>39</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
       <c r="D52" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D53" s="9" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Deckbox Upgrade 2.0 to IP67 (#2)
Update instruction for assembly of deckbox 2.0
* Update README.md
* added images for updated instructions
* Update BOM and Tools
* intructions for USB and Molex Plug
Updated BOM.xlsx
Updated all CAD files to new Deckbox Version
Deleted old images

---------

Co-authored-by: sw-of <sascha.winkler@thuenen.de>
Co-authored-by: Mathis Mahler <mathis.mahler@thuenen.de>
</commit_message>
<xml_diff>
--- a/02_Deckbox/01_Hardware/BOM.xlsx
+++ b/02_Deckbox/01_Hardware/BOM.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD49A64F-274E-4481-B3DF-15A9EA6750CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B530254-4359-491B-B379-8E9E31B77AF6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-14508" yWindow="-7908" windowWidth="14616" windowHeight="22536" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="BOM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="103">
   <si>
     <t>#</t>
   </si>
@@ -40,24 +40,12 @@
     <t>pc</t>
   </si>
   <si>
-    <t>Rittal-PK-9548.000 Mounting plate</t>
-  </si>
-  <si>
     <t>for power supply of router</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>to attach router and raspb. to mouting plate (von Andreas)</t>
-  </si>
-  <si>
-    <t>Dremel/ Drilling machine small</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Reader for micro SD card </t>
-  </si>
-  <si>
     <t>for power supply of Pi</t>
   </si>
   <si>
@@ -76,18 +64,6 @@
     <t>Mounting for box on reeling</t>
   </si>
   <si>
-    <t>Hexagonal screw, M4x16, incl. washer and self-securing nut, stainless steel V4A</t>
-  </si>
-  <si>
-    <t>Steel strap for tubes, DIN 3570, nominal width 46 mm, incl. 2 M10 self-securing nuts and 2 M10 washers, stainless steel V4A</t>
-  </si>
-  <si>
-    <t>Steel strap for tubes, DIN 3570, nominal width 82 mm, incl. 2 M12 self-securing nuts and 2 M12 washers, stainless steel V4A</t>
-  </si>
-  <si>
-    <t>Rittal-PK-9518.000 Case 182x180x111 (Art.-Nr.: W84179)</t>
-  </si>
-  <si>
     <t>External power supply</t>
   </si>
   <si>
@@ -130,12 +106,6 @@
     <t xml:space="preserve">product numbers 0039039042 430300038 </t>
   </si>
   <si>
-    <t>e.g. 4064161155296</t>
-  </si>
-  <si>
-    <t>USB C plug, rectangular, e.g. cut from cable</t>
-  </si>
-  <si>
     <t>2050005621999</t>
   </si>
   <si>
@@ -193,51 +163,18 @@
     <t>for merging incoming power sources</t>
   </si>
   <si>
-    <t>4028177139657</t>
-  </si>
-  <si>
-    <t>4028177140097</t>
-  </si>
-  <si>
-    <t>3D printed mounting for electronic components</t>
-  </si>
-  <si>
     <t>3D printed mounting for antennas of RUT955, consisting of three layers</t>
   </si>
   <si>
     <t>Tools</t>
   </si>
   <si>
-    <t>Drilling machines for 2 mm and 21 mm holes</t>
-  </si>
-  <si>
     <t>e.g. ASIN B09B7F2XM3 or 4260528721160</t>
   </si>
   <si>
-    <t>Threaded inserts to melt into 3D print, M3x6x5</t>
-  </si>
-  <si>
-    <t>Tapping screw (Belchschraube) M2,9x9,5</t>
-  </si>
-  <si>
-    <t>4043377162205</t>
-  </si>
-  <si>
-    <t>Tapping screw (Belchschraube) M2,2x9,5</t>
-  </si>
-  <si>
     <t>4043377159625</t>
   </si>
   <si>
-    <t>Tapping screw (Belchschraube) M3,9x9,5</t>
-  </si>
-  <si>
-    <t>~25</t>
-  </si>
-  <si>
-    <t>Hexagonal screws M3x16</t>
-  </si>
-  <si>
     <t>4043952396568</t>
   </si>
   <si>
@@ -247,12 +184,6 @@
     <t>4043952537589</t>
   </si>
   <si>
-    <t xml:space="preserve">Sealing tape for water tightness </t>
-  </si>
-  <si>
-    <t>Wire 15 cm, 2 x ~0.75mm², red and black</t>
-  </si>
-  <si>
     <t>Soldering station, including equipment e.g. shrinking tubes</t>
   </si>
   <si>
@@ -272,6 +203,133 @@
   </si>
   <si>
     <t>ACDC converter, 12 or 24 V output, min 20 W, e.g. Mean Well LPV-20-12 LED Trafo</t>
+  </si>
+  <si>
+    <t>2-core wire ~25 cm, 2 x ~0.5mm², red and black</t>
+  </si>
+  <si>
+    <t>electric wire ferrule 0.5mm²</t>
+  </si>
+  <si>
+    <t>Heat shrink tubing 20mm x 3mm</t>
+  </si>
+  <si>
+    <t>USB-C Plug, e.g. recable USB C to C plug 5 strands set (consits of 3 parts: plug, housing and heat shrink tubing)</t>
+  </si>
+  <si>
+    <t>FIBOX Case 180x180x150 (Product-No.: 6011323)</t>
+  </si>
+  <si>
+    <t>3D printed mounting for electronic components, consisting of four parts</t>
+  </si>
+  <si>
+    <t>6418074052216</t>
+  </si>
+  <si>
+    <t>Threaded inserts to melt into 3D print, M3x5x4</t>
+  </si>
+  <si>
+    <t>Allen screws M3x16</t>
+  </si>
+  <si>
+    <t>Tapping screw (Belchschraube) M2.9x9.5</t>
+  </si>
+  <si>
+    <t>Tapping screw (Belchschraube) M2.2x6.5</t>
+  </si>
+  <si>
+    <t>Tapping screw (Belchschraube) M3.9x9.5</t>
+  </si>
+  <si>
+    <t>4043377162199</t>
+  </si>
+  <si>
+    <t>(plastic) washers for 3.9 mm with large outer diameter</t>
+  </si>
+  <si>
+    <t>Allen screw, M4x16, incl. washer and self-securing nut, stainless steel V4A</t>
+  </si>
+  <si>
+    <t>Steel strap for tubes, DIN 3570, nominal width 46 mm, incl. 4 M10 nuts and 2 M10 washers, stainless steel V4A</t>
+  </si>
+  <si>
+    <t>Steel strap for tubes, DIN 3570, nominal width 82 mm, incl. 4 M12 nuts and 2 M12 washers, stainless steel V4A</t>
+  </si>
+  <si>
+    <t>Drilling machines 22 mm holes</t>
+  </si>
+  <si>
+    <t>Adapter tip for melting in press nuts</t>
+  </si>
+  <si>
+    <t>Tweezers</t>
+  </si>
+  <si>
+    <t>Diagonal pliers</t>
+  </si>
+  <si>
+    <t>wire stripper</t>
+  </si>
+  <si>
+    <t>Heat gun</t>
+  </si>
+  <si>
+    <t>Wrench 27 mm</t>
+  </si>
+  <si>
+    <t>Allen wrench 2.5 and 3 mm</t>
+  </si>
+  <si>
+    <t>Screwdriver PH1 + PH2</t>
+  </si>
+  <si>
+    <t>Screwdriver flathead (2.5)</t>
+  </si>
+  <si>
+    <t>Caliper</t>
+  </si>
+  <si>
+    <t>Sikaflex (e.g. 291i or some other marine certified adhesive sealant)</t>
+  </si>
+  <si>
+    <t>Spatula</t>
+  </si>
+  <si>
+    <t>Crimp-Tools for 2824-20 and for electric wire ferrules</t>
+  </si>
+  <si>
+    <t>Cleaning equipment: ethanol, q-tips, lint-free wipes</t>
+  </si>
+  <si>
+    <t>flat nose pliers</t>
+  </si>
+  <si>
+    <t>4040849567070</t>
+  </si>
+  <si>
+    <t>9900000247027</t>
+  </si>
+  <si>
+    <t>9900000174064</t>
+  </si>
+  <si>
+    <t>4043952175507</t>
+  </si>
+  <si>
+    <t>4043952665589
+4001796381737</t>
+  </si>
+  <si>
+    <t>4260396830346</t>
+  </si>
+  <si>
+    <t>4043377065032</t>
+  </si>
+  <si>
+    <t>9900000247645</t>
+  </si>
+  <si>
+    <t>~5 cm foam tape (20x2 mm)</t>
   </si>
 </sst>
 </file>
@@ -344,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -378,9 +436,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
@@ -661,21 +716,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G53"/>
+  <dimension ref="A1:G68"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="3" width="4.3984375" customWidth="1"/>
-    <col min="4" max="4" width="64.73046875" style="9" customWidth="1"/>
-    <col min="5" max="5" width="22.3984375" style="15" customWidth="1"/>
-    <col min="6" max="6" width="16.1328125" customWidth="1"/>
+    <col min="1" max="3" width="4.42578125" customWidth="1"/>
+    <col min="4" max="4" width="64.7109375" style="9" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="15" customWidth="1"/>
+    <col min="6" max="6" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:7" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -689,23 +744,23 @@
         <v>3</v>
       </c>
       <c r="E1" s="12" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="8"/>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
       <c r="D2" s="11" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
       <c r="E2" s="13"/>
       <c r="F2" s="8"/>
     </row>
-    <row r="3" spans="1:7" s="3" customFormat="1" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:7" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -716,15 +771,15 @@
         <v>5</v>
       </c>
       <c r="D3" s="7" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="E3" s="14" t="s">
-        <v>29</v>
+        <v>21</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="5"/>
     </row>
-    <row r="4" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -735,13 +790,13 @@
         <v>5</v>
       </c>
       <c r="D4" s="7" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E4" s="14" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -752,10 +807,10 @@
         <v>5</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>4</v>
       </c>
@@ -766,20 +821,20 @@
         <v>5</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="E6" s="15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
       <c r="D7" s="11" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="E7" s="13"/>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>5</v>
       </c>
@@ -790,16 +845,16 @@
         <v>5</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>80</v>
+        <v>57</v>
       </c>
       <c r="E8" s="15" t="s">
-        <v>79</v>
+        <v>56</v>
       </c>
       <c r="F8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>6</v>
       </c>
@@ -810,34 +865,34 @@
         <v>5</v>
       </c>
       <c r="D9" s="7" t="s">
-        <v>83</v>
+        <v>60</v>
       </c>
       <c r="E9" s="14" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>7</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10">
         <v>1</v>
       </c>
       <c r="C10" s="6" t="s">
         <v>5</v>
       </c>
       <c r="D10" s="7" t="s">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="E10" s="14" t="s">
-        <v>34</v>
+        <v>26</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="G10" s="5"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="6">
         <v>8</v>
       </c>
@@ -848,10 +903,10 @@
         <v>5</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>9</v>
       </c>
@@ -862,63 +917,76 @@
         <v>5</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>81</v>
+        <v>58</v>
       </c>
       <c r="E12" s="15" t="s">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G12" s="4"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>10</v>
       </c>
-      <c r="B13" s="6">
-        <v>1</v>
-      </c>
-      <c r="C13" s="6" t="s">
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13" t="s">
         <v>5</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>61</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="F13" s="4"/>
+      <c r="G13" s="4"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>11</v>
       </c>
-      <c r="B14" s="6">
-        <v>1</v>
-      </c>
-      <c r="C14" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D14" s="7" t="s">
-        <v>76</v>
-      </c>
-      <c r="E14" s="14"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A15" s="5"/>
-      <c r="D15" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="E15" s="13"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="B14">
+        <v>6</v>
+      </c>
+      <c r="C14" t="s">
+        <v>5</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="F14" s="4"/>
+      <c r="G14" s="4"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="6">
+        <v>12</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15" t="s">
+        <v>5</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -927,22 +995,20 @@
         <v>5</v>
       </c>
       <c r="D16" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="6"/>
+      <c r="D17" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="E16" s="14" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A17" s="5"/>
-      <c r="D17" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="E17" s="14"/>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.45">
+      <c r="E17" s="13"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -951,30 +1017,20 @@
         <v>5</v>
       </c>
       <c r="D18" s="7" t="s">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="E18" s="14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A19" s="6">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>5</v>
-      </c>
-      <c r="D19" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E19" s="16" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.45">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5"/>
+      <c r="D19" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>15</v>
       </c>
@@ -985,13 +1041,13 @@
         <v>5</v>
       </c>
       <c r="D20" s="7" t="s">
-        <v>49</v>
+        <v>33</v>
       </c>
       <c r="E20" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.45">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>16</v>
       </c>
@@ -1002,13 +1058,13 @@
         <v>5</v>
       </c>
       <c r="D21" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="E21" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.45">
+        <v>37</v>
+      </c>
+      <c r="E21" s="16" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>17</v>
       </c>
@@ -1019,22 +1075,32 @@
         <v>5</v>
       </c>
       <c r="D22" s="7" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="E22" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A23" s="5"/>
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="6">
+        <v>18</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>5</v>
+      </c>
       <c r="D23" s="7" t="s">
-        <v>55</v>
-      </c>
-      <c r="E23" s="14"/>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.45">
+        <v>41</v>
+      </c>
+      <c r="E23" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B24">
         <v>1</v>
@@ -1046,61 +1112,51 @@
         <v>42</v>
       </c>
       <c r="E24" s="14" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A25" s="6">
-        <v>19</v>
-      </c>
-      <c r="B25">
-        <v>1</v>
-      </c>
-      <c r="C25" t="s">
-        <v>5</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.45">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="6"/>
+      <c r="D25" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="E25" s="14"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" s="6">
         <v>20</v>
       </c>
       <c r="B26">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C26" t="s">
         <v>5</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>49</v>
+        <v>32</v>
       </c>
       <c r="E26" s="14" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.45">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27" s="6">
         <v>21</v>
       </c>
       <c r="B27">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C27" t="s">
         <v>5</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="E27" s="14" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.45">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>22</v>
       </c>
@@ -1111,24 +1167,33 @@
         <v>5</v>
       </c>
       <c r="D28" s="7" t="s">
-        <v>53</v>
-      </c>
-      <c r="E28" s="14"/>
-    </row>
-    <row r="29" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="8"/>
-      <c r="B29" s="8"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="E28" s="14" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="6">
+        <v>23</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29" t="s">
+        <v>5</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="E29" s="14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="6">
         <v>24</v>
       </c>
-      <c r="E29" s="13"/>
-      <c r="F29" s="8"/>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A30" s="6">
-        <v>23</v>
-      </c>
       <c r="B30">
         <v>1</v>
       </c>
@@ -1136,49 +1201,39 @@
         <v>5</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="14" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.45">
-      <c r="A31" s="6">
-        <v>24</v>
-      </c>
-      <c r="B31">
-        <v>1</v>
-      </c>
-      <c r="C31" t="s">
-        <v>5</v>
-      </c>
-      <c r="D31" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="E31" s="14" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="5">
+        <v>43</v>
+      </c>
+      <c r="E30" s="14"/>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="E31" s="13"/>
+      <c r="F31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="6">
         <v>25</v>
       </c>
-      <c r="B32" s="5">
-        <v>1</v>
-      </c>
-      <c r="C32" s="5" t="s">
+      <c r="B32">
+        <v>1</v>
+      </c>
+      <c r="C32" t="s">
         <v>5</v>
       </c>
       <c r="D32" s="7" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="E32" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="F32" s="8"/>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A33" s="6">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" s="3" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="5">
         <v>26</v>
       </c>
       <c r="B33">
@@ -1188,141 +1243,158 @@
         <v>5</v>
       </c>
       <c r="D33" s="9" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="E33" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="34" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+        <v>56</v>
+      </c>
+      <c r="F33" s="8"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="6">
         <v>27</v>
       </c>
       <c r="B34">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C34" t="s">
         <v>5</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>64</v>
-      </c>
-      <c r="E34" s="15" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.45">
+        <v>47</v>
+      </c>
+      <c r="E34" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="6">
         <v>28</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C35" t="s">
         <v>5</v>
       </c>
       <c r="D35" s="9" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.45">
+        <v>68</v>
+      </c>
+      <c r="E35" s="15" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>29</v>
       </c>
       <c r="B36">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
         <v>5</v>
       </c>
       <c r="D36" s="9" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.45">
+        <v>69</v>
+      </c>
+      <c r="E36" s="13" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="6">
         <v>30</v>
       </c>
       <c r="B37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C37" t="s">
         <v>5</v>
       </c>
-      <c r="D37" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="E37" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="F37" t="s">
-        <v>9</v>
-      </c>
-      <c r="G37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D37" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E37" s="13" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="6">
         <v>31</v>
       </c>
-      <c r="B38" s="17" t="s">
-        <v>70</v>
+      <c r="B38">
+        <v>2</v>
       </c>
       <c r="C38" t="s">
         <v>5</v>
       </c>
       <c r="D38" s="7" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="E38" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G38" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.45">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>32</v>
       </c>
       <c r="B39">
-        <v>2</v>
+        <v>28</v>
       </c>
       <c r="C39" t="s">
         <v>5</v>
       </c>
       <c r="D39" s="7" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="E39" s="14" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" x14ac:dyDescent="0.45">
+        <v>53</v>
+      </c>
+      <c r="G39" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="6">
         <v>33</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C40" t="s">
         <v>5</v>
       </c>
-      <c r="D40" s="9" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A41" s="5"/>
-      <c r="D41" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="E41" s="13"/>
-    </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="D40" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="E40" s="14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="6">
+        <v>34</v>
+      </c>
+      <c r="B41">
+        <v>4</v>
+      </c>
+      <c r="C41" t="s">
+        <v>5</v>
+      </c>
+      <c r="D41" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="E41" s="13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="6">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1330,89 +1402,180 @@
       <c r="C42" t="s">
         <v>5</v>
       </c>
-      <c r="D42" s="7" t="s">
-        <v>78</v>
-      </c>
-      <c r="E42" s="14" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A43" s="6">
-        <v>35</v>
-      </c>
-      <c r="B43">
-        <v>4</v>
-      </c>
-      <c r="C43" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="E43" s="14"/>
-    </row>
-    <row r="44" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D42" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="E42" s="13" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="13.9" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="5"/>
+      <c r="D43" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="E43" s="13"/>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="6">
         <v>36</v>
       </c>
       <c r="B44">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C44" t="s">
         <v>5</v>
       </c>
-      <c r="D44" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="E44" s="15" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="45" spans="1:7" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="D44" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E44" s="14" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="6">
         <v>37</v>
       </c>
       <c r="B45">
+        <v>4</v>
+      </c>
+      <c r="C45" t="s">
+        <v>5</v>
+      </c>
+      <c r="D45" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="E45" s="13" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="6">
+        <v>38</v>
+      </c>
+      <c r="B46">
         <v>2</v>
       </c>
-      <c r="C45" t="s">
-        <v>5</v>
-      </c>
-      <c r="D45" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="E45" s="15" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A46" s="5"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.45">
-      <c r="A47" s="5"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A50" t="s">
-        <v>61</v>
-      </c>
-      <c r="D50" s="9" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="D51" s="9" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C46" t="s">
+        <v>5</v>
+      </c>
+      <c r="D46" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E46" s="15" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="6">
+        <v>39</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47" t="s">
+        <v>5</v>
+      </c>
+      <c r="D47" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="E47" s="15" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="5"/>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="5"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>48</v>
+      </c>
       <c r="D52" s="9" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.45">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D53" s="9" t="s">
-        <v>11</v>
+        <v>54</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D54" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D55" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D56" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D57" s="9" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D58" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D59" s="9" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D60" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D61" s="9" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D62" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D63" s="9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D64" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D65" s="9" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="66" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D66" s="9" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="67" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D67" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="68" spans="4:4" x14ac:dyDescent="0.25">
+      <c r="D68" s="9" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>